<commit_message>
edit tables name without 's'
</commit_message>
<xml_diff>
--- a/doc/BLOG_ERD_Design.xlsx
+++ b/doc/BLOG_ERD_Design.xlsx
@@ -53,24 +53,12 @@
     <t>modified_at</t>
   </si>
   <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>users</t>
-  </si>
-  <si>
-    <t>posts</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
     <t>BLOG-ERD-DESIGN</t>
   </si>
   <si>
-    <t>ENTITY :USERS</t>
-  </si>
-  <si>
     <t>User id</t>
   </si>
   <si>
@@ -95,9 +83,6 @@
     <t>First name</t>
   </si>
   <si>
-    <t>ENTITY :POSTS</t>
-  </si>
-  <si>
     <t>Post id</t>
   </si>
   <si>
@@ -131,9 +116,6 @@
     <t>Date time of the post modified</t>
   </si>
   <si>
-    <t>ENTITY :COMMENTS</t>
-  </si>
-  <si>
     <t>Comment id</t>
   </si>
   <si>
@@ -153,6 +135,27 @@
   </si>
   <si>
     <t>Tables</t>
+  </si>
+  <si>
+    <t>(0,n)</t>
+  </si>
+  <si>
+    <t>ENTITY :USER</t>
+  </si>
+  <si>
+    <t>ENTITY :POST</t>
+  </si>
+  <si>
+    <t>ENTITY :COMMENT</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>comment</t>
   </si>
   <si>
     <r>
@@ -164,7 +167,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>users</t>
+      <t>user</t>
     </r>
     <r>
       <rPr>
@@ -187,7 +190,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>posts</t>
+      <t>post</t>
     </r>
     <r>
       <rPr>
@@ -210,7 +213,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>comments</t>
+      <t>comment</t>
     </r>
     <r>
       <rPr>
@@ -222,9 +225,6 @@
       </rPr>
       <t>(id, content, created_at, modified_at, author_id, post_id)</t>
     </r>
-  </si>
-  <si>
-    <t>(0,n)</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1111,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A32:A38" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="A32:A38"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="users"/>
+    <tableColumn id="1" name="user"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1121,7 +1121,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="D37:D41" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1">
   <autoFilter ref="D37:D41"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="comments"/>
+    <tableColumn id="1" name="comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1131,7 +1131,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="D28:D33" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4">
   <autoFilter ref="D28:D33"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="posts"/>
+    <tableColumn id="1" name="post"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1402,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,7 +1446,7 @@
     </row>
     <row r="2" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="31" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="32"/>
       <c r="C2" s="32"/>
@@ -1470,7 +1470,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
@@ -1479,33 +1479,33 @@
     </row>
     <row r="5" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>1</v>
@@ -1516,7 +1516,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>2</v>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>3</v>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>4</v>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="15"/>
@@ -1565,52 +1565,52 @@
     </row>
     <row r="13" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -1618,13 +1618,13 @@
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B19" s="34"/>
       <c r="C19" s="35"/>
@@ -1650,13 +1650,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -1664,13 +1664,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -1678,13 +1678,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -1692,13 +1692,13 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -1727,12 +1727,12 @@
     </row>
     <row r="28" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D28" s="6" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D29" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1740,12 +1740,12 @@
         <v>5</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="17" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>6</v>
@@ -1753,18 +1753,18 @@
     </row>
     <row r="32" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>8</v>
@@ -1790,10 +1790,10 @@
         <v>3</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1801,13 +1801,13 @@
         <v>4</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F38" s="17"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C39" s="17" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>6</v>
@@ -1815,10 +1815,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D40" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1831,7 +1831,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B43" s="21"/>
       <c r="C43" s="21"/>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="44" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" s="23"/>
       <c r="C44" s="23"/>
@@ -1848,7 +1848,7 @@
     </row>
     <row r="45" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" s="26"/>
       <c r="C45" s="26"/>
@@ -1856,7 +1856,7 @@
     </row>
     <row r="46" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" s="29"/>
       <c r="C46" s="29"/>

</xml_diff>